<commit_message>
added print array and list
</commit_message>
<xml_diff>
--- a/Quotes.xlsx
+++ b/Quotes.xlsx
@@ -1,22 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20515"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="165" windowWidth="14355" windowHeight="6150"/>
+    <workbookView xWindow="-20480" yWindow="-5020" windowWidth="25940" windowHeight="17840"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="92">
   <si>
     <t>You lily livered yellow bellied scroundrel.</t>
   </si>
@@ -283,13 +288,22 @@
   </si>
   <si>
     <t>New York city! Get a rope.</t>
+  </si>
+  <si>
+    <t>I'm Buford 'Pi' Tannen</t>
+  </si>
+  <si>
+    <t>Blargh! *DEATH*</t>
+  </si>
+  <si>
+    <t>I call my gun Vera</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -309,6 +323,22 @@
     </font>
     <font>
       <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -400,7 +430,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -410,22 +440,22 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -435,7 +465,7 @@
     <border>
       <left/>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -443,126 +473,126 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -570,91 +600,320 @@
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="medium">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="219">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -717,8 +976,227 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="219">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1018,21 +1496,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B63"/>
+  <dimension ref="A1:B66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="B48" sqref="B48"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="110.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" customWidth="1"/>
-    <col min="4" max="4" width="77.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="110.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" customWidth="1"/>
+    <col min="4" max="4" width="77.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="17" t="s">
         <v>28</v>
       </c>
@@ -1040,61 +1518,61 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2">
       <c r="A2" s="18"/>
       <c r="B2" s="5" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2">
       <c r="A3" s="18"/>
       <c r="B3" s="5" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2">
       <c r="A4" s="18"/>
       <c r="B4" s="12" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2">
       <c r="A5" s="18"/>
       <c r="B5" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2">
       <c r="A6" s="18"/>
       <c r="B6" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2">
       <c r="A7" s="18"/>
       <c r="B7" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2">
       <c r="A8" s="18"/>
       <c r="B8" s="5" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2">
       <c r="A9" s="18"/>
       <c r="B9" s="5" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" ht="15" thickBot="1">
       <c r="A10" s="19"/>
       <c r="B10" s="7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2">
       <c r="A11" s="23" t="s">
         <v>24</v>
       </c>
@@ -1102,19 +1580,19 @@
         <v>25</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2">
       <c r="A12" s="15"/>
       <c r="B12" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" ht="15" thickBot="1">
       <c r="A13" s="16"/>
       <c r="B13" s="7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2">
       <c r="A14" s="21" t="s">
         <v>29</v>
       </c>
@@ -1122,19 +1600,19 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2">
       <c r="A15" s="22"/>
       <c r="B15" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" ht="15" thickBot="1">
       <c r="A16" s="22"/>
       <c r="B16" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" ht="15">
       <c r="A17" s="8" t="s">
         <v>33</v>
       </c>
@@ -1142,7 +1620,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" ht="15">
       <c r="A18" s="9" t="s">
         <v>35</v>
       </c>
@@ -1150,7 +1628,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2">
       <c r="A19" s="57" t="s">
         <v>37</v>
       </c>
@@ -1158,7 +1636,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" ht="15">
       <c r="A20" s="9" t="s">
         <v>39</v>
       </c>
@@ -1166,7 +1644,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" ht="16" thickBot="1">
       <c r="A21" s="10" t="s">
         <v>41</v>
       </c>
@@ -1174,7 +1652,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" ht="16" thickBot="1">
       <c r="A22" s="52" t="s">
         <v>63</v>
       </c>
@@ -1182,7 +1660,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" ht="16" thickBot="1">
       <c r="A23" s="26" t="s">
         <v>45</v>
       </c>
@@ -1190,7 +1668,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" ht="15">
       <c r="A24" s="28" t="s">
         <v>47</v>
       </c>
@@ -1198,25 +1676,25 @@
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2">
       <c r="A25" s="29"/>
       <c r="B25" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2">
       <c r="A26" s="29"/>
       <c r="B26" s="5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" ht="15" thickBot="1">
       <c r="A27" s="30"/>
       <c r="B27" s="7" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2">
       <c r="A28" s="46" t="s">
         <v>50</v>
       </c>
@@ -1224,19 +1702,19 @@
         <v>49</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2">
       <c r="A29" s="40"/>
       <c r="B29" s="37" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="30" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" ht="15" thickBot="1">
       <c r="A30" s="35"/>
       <c r="B30" s="33" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2">
       <c r="A31" s="24" t="s">
         <v>44</v>
       </c>
@@ -1244,67 +1722,67 @@
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2">
       <c r="A32" s="25"/>
       <c r="B32" s="5" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:2">
       <c r="A33" s="25"/>
       <c r="B33" s="5" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:2">
       <c r="A34" s="25"/>
       <c r="B34" s="13" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:2">
       <c r="A35" s="25"/>
       <c r="B35" s="5" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:2">
       <c r="A36" s="25"/>
       <c r="B36" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:2">
       <c r="A37" s="25"/>
       <c r="B37" s="5" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:2">
       <c r="A38" s="25"/>
       <c r="B38" s="5" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:2">
       <c r="A39" s="59"/>
       <c r="B39" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:2">
       <c r="A40" s="59"/>
       <c r="B40" s="1" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" ht="15" thickBot="1">
       <c r="A41" s="36"/>
       <c r="B41" s="31" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:2">
       <c r="A42" s="38" t="s">
         <v>52</v>
       </c>
@@ -1312,19 +1790,19 @@
         <v>53</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:2">
       <c r="A43" s="39"/>
       <c r="B43" s="37" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" ht="15" thickBot="1">
       <c r="A44" s="41"/>
       <c r="B44" s="42" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:2">
       <c r="A45" s="43" t="s">
         <v>55</v>
       </c>
@@ -1332,19 +1810,19 @@
         <v>56</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:2">
       <c r="A46" s="45"/>
       <c r="B46" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" ht="15" thickBot="1">
       <c r="A47" s="44"/>
       <c r="B47" s="33" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:2">
       <c r="A48" s="53" t="s">
         <v>60</v>
       </c>
@@ -1352,13 +1830,13 @@
         <v>61</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" ht="15" thickBot="1">
       <c r="A49" s="54"/>
       <c r="B49" s="31" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" ht="15" thickBot="1">
       <c r="A50" s="50" t="s">
         <v>59</v>
       </c>
@@ -1366,7 +1844,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" ht="15" thickBot="1">
       <c r="A51" s="56" t="s">
         <v>65</v>
       </c>
@@ -1374,7 +1852,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" ht="15" thickBot="1">
       <c r="A52" s="48" t="s">
         <v>66</v>
       </c>
@@ -1382,7 +1860,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" ht="15" thickBot="1">
       <c r="A53" s="56" t="s">
         <v>67</v>
       </c>
@@ -1390,7 +1868,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" ht="15" thickBot="1">
       <c r="A54" s="48" t="s">
         <v>68</v>
       </c>
@@ -1398,7 +1876,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:2">
       <c r="A55" s="14" t="s">
         <v>69</v>
       </c>
@@ -1406,7 +1884,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" ht="15" thickBot="1">
       <c r="A56" s="16" t="s">
         <v>71</v>
       </c>
@@ -1414,7 +1892,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:2">
       <c r="A57" s="20" t="s">
         <v>70</v>
       </c>
@@ -1422,7 +1900,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" ht="15" thickBot="1">
       <c r="A58" s="55" t="s">
         <v>71</v>
       </c>
@@ -1430,7 +1908,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:2">
       <c r="A59" s="34" t="s">
         <v>82</v>
       </c>
@@ -1438,13 +1916,13 @@
         <v>83</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" ht="15" thickBot="1">
       <c r="A60" s="58"/>
       <c r="B60" s="42" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:2">
       <c r="A61" s="2" t="s">
         <v>27</v>
       </c>
@@ -1452,21 +1930,41 @@
         <v>86</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:2">
       <c r="A62" s="4"/>
       <c r="B62" s="37" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" ht="15" thickBot="1">
       <c r="A63" s="6"/>
       <c r="B63" s="33" t="s">
         <v>87</v>
       </c>
     </row>
+    <row r="64" spans="1:2">
+      <c r="B64" s="60" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2">
+      <c r="B65" s="60" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2">
+      <c r="B66" s="60" t="s">
+        <v>91</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" verticalDpi="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1476,9 +1974,14 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -1488,8 +1991,13 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>